<commit_message>
Backend Conectando a MongoDB
Este commit muestra como instalar el driver de mongodb, actualizar el archivo www para conectar a la db , modificar app.js para que exponga una función donde se pueda inyectar la conección establecida de mongodb, crear una ruta (inyectable) para sacar la información de una colección.
</commit_message>
<xml_diff>
--- a/DOCS/API_ANALSIS.xlsx
+++ b/DOCS/API_ANALSIS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/obetancourth/Documents/CLASES_SCJ/SW/202001/lencaStore/DOCS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C971BF6B-8185-2546-936D-3B7442754AFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4410B598-3958-9940-A908-D75D976BF724}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{9720F37F-D650-1649-ACD0-78AE281E3002}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" xr2:uid="{9720F37F-D650-1649-ACD0-78AE281E3002}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="94">
   <si>
     <t>ENTIDADES</t>
   </si>
@@ -300,6 +300,21 @@
   </si>
   <si>
     <t>UC0019</t>
+  </si>
+  <si>
+    <t>MongoDBCollection</t>
+  </si>
+  <si>
+    <t>productos</t>
+  </si>
+  <si>
+    <t>PseudoSchema</t>
+  </si>
+  <si>
+    <t>sku, descripcion, descripcioncorta, metodoenvio, stock, urlfoto, precio, categorias, historicoprecios, estado</t>
+  </si>
+  <si>
+    <t>ordenes</t>
   </si>
 </sst>
 </file>
@@ -408,11 +423,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{47045FBD-73FF-3D46-8769-39B18210BF9C}" name="Table1" displayName="Table1" ref="A1:I23" totalsRowShown="0">
-  <autoFilter ref="A1:I23" xr:uid="{748DE1ED-A284-5742-A0F2-93B94F015A17}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{FA7003C4-FDEA-C249-985B-5C17D37E8F31}" name="ENTIDADES" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{A12D6747-794C-9F4D-B52C-136B73CAC69B}" name="Casos" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{47045FBD-73FF-3D46-8769-39B18210BF9C}" name="Table1" displayName="Table1" ref="A1:K23" totalsRowShown="0">
+  <autoFilter ref="A1:K23" xr:uid="{748DE1ED-A284-5742-A0F2-93B94F015A17}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{FA7003C4-FDEA-C249-985B-5C17D37E8F31}" name="ENTIDADES" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{A12D6747-794C-9F4D-B52C-136B73CAC69B}" name="Casos" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{8F6FA4F1-E359-6345-861F-9CD9062F880D}" name="Acceso"/>
     <tableColumn id="4" xr3:uid="{CB715C32-9DFE-1347-B5F3-107B6A7720F8}" name="Ruta"/>
     <tableColumn id="5" xr3:uid="{F000BFF0-6D64-9E40-A7F6-F5EEA44737D7}" name="Metodo"/>
@@ -420,6 +435,8 @@
     <tableColumn id="7" xr3:uid="{F982D592-5512-4549-8305-03B60B367A09}" name="Body" dataDxfId="0"/>
     <tableColumn id="8" xr3:uid="{909EFD11-46F8-CF44-B818-132AC3DA407F}" name="Status"/>
     <tableColumn id="9" xr3:uid="{CAE6380A-30D7-7943-A6EE-61A8F740FE95}" name="Use Case Map"/>
+    <tableColumn id="10" xr3:uid="{EC9C60E4-305B-834F-AEEA-08EEF862047E}" name="MongoDBCollection"/>
+    <tableColumn id="11" xr3:uid="{7F9A049E-CD0A-3E47-8147-E7F8F2B13D5E}" name="PseudoSchema"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -722,10 +739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2001497-AD5D-6F4D-8D38-71092A6BDF46}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -734,9 +751,10 @@
     <col min="2" max="2" width="30.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="30.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="30.1640625" customWidth="1"/>
+    <col min="11" max="11" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -764,14 +782,20 @@
       <c r="I1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="44" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="44" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>24</v>
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -794,7 +818,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="85" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>42</v>
       </c>
@@ -814,8 +838,14 @@
       <c r="I4" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J4" t="s">
+        <v>90</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
@@ -835,8 +865,11 @@
       <c r="I5" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="J5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
@@ -861,8 +894,11 @@
       <c r="I6" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>33</v>
       </c>
@@ -887,8 +923,11 @@
       <c r="I7" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>22</v>
       </c>
@@ -911,8 +950,11 @@
       <c r="I8" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>25</v>
       </c>
@@ -932,8 +974,11 @@
       <c r="I9" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>28</v>
       </c>
@@ -955,8 +1000,11 @@
       <c r="I10" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="J10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>31</v>
       </c>
@@ -978,8 +1026,11 @@
       <c r="I11" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="44" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="44" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>1</v>
       </c>
@@ -990,7 +1041,7 @@
       <c r="F12" s="5"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>37</v>
       </c>
@@ -1013,7 +1064,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>36</v>
       </c>
@@ -1034,7 +1085,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>44</v>
       </c>
@@ -1057,7 +1108,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
Backlog add artesanos api
</commit_message>
<xml_diff>
--- a/DOCS/API_ANALSIS.xlsx
+++ b/DOCS/API_ANALSIS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/obetancourth/Documents/CLASES_SCJ/SW/202001/lencaStore/DOCS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4410B598-3958-9940-A908-D75D976BF724}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EAB48CC-9695-9C49-82B2-8F6907B0D317}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" xr2:uid="{9720F37F-D650-1649-ACD0-78AE281E3002}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="95">
   <si>
     <t>ENTIDADES</t>
   </si>
@@ -315,6 +315,9 @@
   </si>
   <si>
     <t>ordenes</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -741,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2001497-AD5D-6F4D-8D38-71092A6BDF46}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -833,7 +836,7 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="I4" t="s">
         <v>71</v>
@@ -860,7 +863,7 @@
       </c>
       <c r="G5" s="1"/>
       <c r="H5" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="I5" t="s">
         <v>72</v>
@@ -889,7 +892,7 @@
         <v>21</v>
       </c>
       <c r="H6" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="I6" t="s">
         <v>73</v>
@@ -918,7 +921,7 @@
         <v>35</v>
       </c>
       <c r="H7" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="I7" t="s">
         <v>74</v>
@@ -945,7 +948,7 @@
       </c>
       <c r="G8" s="1"/>
       <c r="H8" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="I8" t="s">
         <v>75</v>

</xml_diff>